<commit_message>
Upload completed lab 5
</commit_message>
<xml_diff>
--- a/lab5/statetable.xlsx
+++ b/lab5/statetable.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UCSB IEEE\Documents\alu-repos\ece152a\lab5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\GitHub\ece152a\lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F8FC46-77EB-495B-A55E-BB276B0D19F5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB6508A-BB20-4DE6-8E84-14B6E038BB63}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="7980" xr2:uid="{C111D1D0-9ED6-45DE-A88B-68A13C65E49B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C111D1D0-9ED6-45DE-A88B-68A13C65E49B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -189,18 +195,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -518,7 +517,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,10 +1076,10 @@
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>13</v>
@@ -1099,7 +1098,7 @@
       </c>
       <c r="L16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>11'bxxxxxx0xx11: cs = 6'b111111;</v>
+        <v>11'bxxxxxx00011: cs = 6'b111111;</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>